<commit_message>
added 64 line xyz...
</commit_message>
<xml_diff>
--- a/Intquestions.xlsx
+++ b/Intquestions.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Interview Question Bank\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A27B2A9-71C1-4CEC-BB71-490E4C045280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F8501268-94FE-4F68-B189-A1E49F48DC16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Nitin Swami - Interview Questions</t>
   </si>
@@ -193,13 +187,16 @@
   </si>
   <si>
     <t>Hello brother this is the third time I am tryin to make a few more changees to the xl file and these changes have been commiteed by Mr Nitin Swami</t>
+  </si>
+  <si>
+    <t>xyz..................................</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -368,7 +365,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -562,81 +559,81 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0856A20-8F21-46B0-8911-E53F0CB9F569}">
-  <dimension ref="A1:B62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="178.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -644,37 +641,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -682,179 +679,184 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>